<commit_message>
CS, database, FI invoice
</commit_message>
<xml_diff>
--- a/QuotationTemplate.xlsx
+++ b/QuotationTemplate.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\C-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314EFCC3-F7EB-4E08-9A22-6DD9D4406F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AC2F17-5058-4818-BDCB-C7FEA5290A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CBF61DC2-AF71-4293-B487-5EE37460939B}"/>
+    <workbookView xWindow="4830" yWindow="2235" windowWidth="21600" windowHeight="11295" xr2:uid="{CBF61DC2-AF71-4293-B487-5EE37460939B}"/>
   </bookViews>
   <sheets>
     <sheet name="Quotation" sheetId="2" r:id="rId1"/>
-    <sheet name="Invoice" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>SMILE &amp; SUNSHINE TOY CO, LTD.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -45,9 +44,6 @@
   <si>
     <t>s&amp;stoy@gmail.com | +852 1234 1234</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Client Email: </t>
   </si>
   <si>
     <t>Date Prepared:</t>
@@ -181,10 +177,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Transprot: </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Unit Price</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -193,11 +185,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Invoice No:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>I</t>
+    <t xml:space="preserve">Transport: </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Address: </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -637,8 +629,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -678,30 +694,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -766,61 +758,6 @@
         <a:xfrm>
           <a:off x="5485209" y="280988"/>
           <a:ext cx="738185" cy="739375"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>494109</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>71438</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>413144</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>67863</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30040AC6-0D4E-B33C-5A3D-3B32FC7A59B4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5328047" y="279797"/>
-          <a:ext cx="740566" cy="740566"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1151,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472DEE5D-96ED-4B29-B590-F6AD3CC7BAA1}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1187,24 +1124,24 @@
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -1232,11 +1169,13 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="22" t="s">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C8" s="24"/>
       <c r="E8" s="22" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
@@ -1247,11 +1186,12 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>3</v>
-      </c>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -1261,11 +1201,13 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="22" t="s">
-        <v>19</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C12" s="24"/>
       <c r="E12" s="22" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
@@ -1277,7 +1219,7 @@
     </row>
     <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
@@ -1289,239 +1231,218 @@
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="45"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="16"/>
       <c r="E17" s="15"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="16"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="16"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="16"/>
       <c r="E20" s="15"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="16"/>
       <c r="E21" s="15"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="16"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="16"/>
       <c r="E23" s="15"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="16"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="17"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
     </row>
     <row r="26" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="17"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
-      <c r="F27" s="29">
+      <c r="F27" s="37">
         <f>SUM(F17:G26)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="30"/>
+      <c r="G27" s="38"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="32"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="40"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
-      <c r="F29" s="31">
+      <c r="F29" s="39">
         <f>F27-F28</f>
         <v>0</v>
       </c>
-      <c r="G29" s="32"/>
+      <c r="G29" s="40"/>
     </row>
     <row r="30" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
+      <c r="B30" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="22" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C32" s="24"/>
       <c r="E32" s="22" t="s">
-        <v>22</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F32" s="24"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C34" s="24"/>
     </row>
     <row r="37" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
+      <c r="B37" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
     </row>
     <row r="38" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+    </row>
+    <row r="39" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-    </row>
-    <row r="39" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
     </row>
     <row r="40" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
     </row>
     <row r="41" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+    </row>
+    <row r="42" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-    </row>
-    <row r="42" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="F26:G26"/>
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="B39:G39"/>
     <mergeCell ref="B41:G41"/>
@@ -1532,6 +1453,30 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="D30:G30"/>
     <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F17:G17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -1541,402 +1486,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E43D46-667F-4F2D-BB21-0AF41B25960C}">
-  <dimension ref="A1:H42"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="8.375" customWidth="1"/>
-    <col min="4" max="4" width="10.625" customWidth="1"/>
-    <col min="5" max="5" width="12.75" customWidth="1"/>
-    <col min="6" max="6" width="10.625" customWidth="1"/>
-    <col min="7" max="7" width="10.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="22"/>
-      <c r="E9" s="23"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="22"/>
-      <c r="E11" s="23"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="45"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-    </row>
-    <row r="26" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="29">
-        <f>SUM(F17:G26)</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="30"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="32"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="31">
-        <f>F27-F28</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="32"/>
-    </row>
-    <row r="30" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-    </row>
-    <row r="38" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-    </row>
-    <row r="39" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-    </row>
-    <row r="40" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="12"/>
-    </row>
-    <row r="41" spans="2:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-    </row>
-    <row r="42" spans="2:7" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-    </row>
-  </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="F26:G26"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{EF549E89-8050-4BEB-9B72-5ECA40451F39}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
-  <drawing r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>